<commit_message>
Mise à jour planning
</commit_message>
<xml_diff>
--- a/QCM_Sicharp/PlanningFinal.xlsx
+++ b/QCM_Sicharp/PlanningFinal.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="23">
   <si>
     <t>7h30</t>
   </si>
@@ -84,15 +84,6 @@
     <t>Processus de suppression de mots-clés</t>
   </si>
   <si>
-    <t>Processus de création de réponses</t>
-  </si>
-  <si>
-    <t>Processus de modification de reponses</t>
-  </si>
-  <si>
-    <t>Processus de suppression de reponses</t>
-  </si>
-  <si>
     <t>Processus d'exportation au format Latex</t>
   </si>
   <si>
@@ -103,6 +94,9 @@
   </si>
   <si>
     <t>Création de la présentation</t>
+  </si>
+  <si>
+    <t>Maquettes</t>
   </si>
 </sst>
 </file>
@@ -119,6 +113,7 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -139,13 +134,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -162,16 +157,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,7 +472,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -489,79 +483,78 @@
   <dimension ref="A2:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" activeCellId="1" sqref="H5:I5 E5:F5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="4"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="6">
+      <c r="B2" s="1">
         <v>42892</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -624,7 +617,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -697,24 +690,24 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -726,7 +719,7 @@
   <dimension ref="A2:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,16 +771,16 @@
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -872,7 +865,7 @@
   <dimension ref="A2:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,7 +925,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -947,10 +940,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L5"/>
+  <dimension ref="A2:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="H4" sqref="H4:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,23 +993,18 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1025,10 +1013,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L4"/>
+  <dimension ref="A2:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="H4" sqref="H4:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1066,91 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <v>42899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1090,84 +1162,6 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="1">
-        <v>42899</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1229,7 +1223,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>

</xml_diff>